<commit_message>
Refactor code structure and improve readability
</commit_message>
<xml_diff>
--- a/output/jobs.xlsx
+++ b/output/jobs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,370 +473,370 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>College Intern</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Hewlett Packard</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ahmedabad,Gurugram</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>Competitive stipend</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/college-intern-internship-in-bangalore-at-hewlett-packard1758536943</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Operations And Strategy</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>EkStep</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 15,000 - 20,000 /month</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/operations-and-strategy-internship-in-bangalore-at-ekstep1762504606</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Business Development Intern</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>PlatinumRx.in</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 15,000 - 25,000 /month</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/partnership-internship-in-bangalore-at-platinumrxin1763702380</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Technical Writer</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>DTALES Tech</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore(Hybrid)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 15,000 /month</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/technical-writer-internship-in-bangalore-at-dtales-tech1764236817</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Digital Marketing</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Chola Apparels</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 5,000 - 8,000 /month</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/digital-marketing-internship-in-bangalore-at-chola-apparels1764163866</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Supply Chain Management (SCM)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Monrow Shoes</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 15,000 /month</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/supply-chain-management-scm-internship-in-bangalore-at-monrow-shoes1764226109</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Data Entry</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>NoBroker</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 12,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/data-entry-internship-in-bangalore-at-nobroker1764254680</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Technical Program Manager</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Razorpay</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>Competitive stipend</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/technical-program-manager-internship-in-bangalore-at-razorpay1764311275</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Content and Social Media Marketing</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Fiscal Flow</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 8,000 - 14,000 /month</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/content-and-social-media-marketing-internship-in-bangalore-at-fiscal-flow1763467186</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Founders Office &amp; Marketing</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>SuperU</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 15,000 - 30,000 /month</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/founders-office-marketing-internship-in-bangalore-at-superu1763461248</t>
         </is>
       </c>
     </row>
@@ -853,22 +853,22 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>⭐ 4.5</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -880,360 +880,360 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Community Activation</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Marzi By Primus</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 15,000 - 20,000 /month</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/community-activation-internship-in-bangalore-at-marzi-by-primus1763551901</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Marketing Research &amp; Analytics</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>CertPro</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 15,000 - 25,000 /month</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/marketing-research-analytics-internship-in-bangalore-at-certpro1763608097</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Customer Service/Customer Support</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>AQ Corporation India Private Limited</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 7,500 - 10,000 /month</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/customer-service-customer-support-internship-in-bangalore-at-aq-corporation-india-private-limited1763556900</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>E-Commerce Operations</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>RuralEquip PVT Ltd</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 8,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/e-commerce-operations-internship-in-bangalore-at-ruralequip-pvt-ltd1764168724</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Content and Social Media Marketing</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Tanai Balaji</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore(Hybrid)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 4,000 - 6,000 /month</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/part-time-content-and-social-media-marketing-internship-in-bangalore-at-tanai-balaji1764226392</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Customer Service/Customer Support</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Sugar.fit</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 15,000 /month</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/customer-service-customer-support-internship-in-bangalore-at-sugarfit1764219786</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Key Account Associate</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>HappyLocate Relocation Services Private Limited</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 10,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/key-account-associate-internship-in-bangalore-at-happylocate-relocation-services-private-limited1764238570</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Telecalling</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Infocruise Solutions Private LImited</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 8,500 - 10,000 /month</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/telecalling-internship-in-bangalore-at-infocruise-solutions-private-limited1764241856</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Event Management</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>NYUC Technologies</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Delhi, Hyderabad, Mumbai, Bangalore(Hybrid)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Not Mentioned</t>
+          <t>₹ 15,000 /month</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/event-management-internship-in-multiple-locations-at-nyuc-technologies1763959180</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Internet Of Things (IoT)</t>
+          <t>Client Servicing</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>DIPC Tech Private Limited</t>
+          <t>WILDFOX BUSINESS ADVOCACY</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>₹ 6,000 - 11,000 /month</t>
+          <t>₹ 2,000 /month</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1243,34 +1243,34 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/internet-of-things-iot-internship-in-ahmedabad-at-dipc-tech-private-limited1763616274</t>
+          <t>https://internshala.com/internship/detail/client-servicing-internship-in-bangalore-at-wildfox-business-advocacy1764689795</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>AI And System Embedded Engineer</t>
+          <t>GTM</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ATSC</t>
+          <t>FirstClub Technology Private Limited</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>₹ 10,000 /month</t>
+          <t>₹ 25,000 - 30,000 /month</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1280,34 +1280,34 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/ai-and-system-embedded-engineer-internship-in-ahmedabad-at-atsc1763380660</t>
+          <t>https://internshala.com/internship/detail/gtm-internship-in-bangalore-at-firstclub-technology-private-limited1764829004</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Information Technology</t>
+          <t>Office Assistant</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ITGS Infotech Private Limited</t>
+          <t>Shree Impex</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore, Koramangala</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>₹ 10,000 - 20,000 /month</t>
+          <t>₹ 2,000 - 7,000 /month</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1317,34 +1317,34 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/part-time-information-technology-internship-in-multiple-locations-at-itgs-infotech-private-limited1764671132</t>
+          <t>https://internshala.com/internship/detail/office-assistant-internship-in-multiple-locations-at-shree-impex1763461455</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Data Annotations For AI Model Training</t>
+          <t>E-Commerce</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Eonian Software Solutions Private Limited</t>
+          <t>Monrow Shoes</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>₹ 2,500 - 4,000 /month</t>
+          <t>₹ 15,000 /month</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1354,34 +1354,34 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/part-time-data-annotations-for-ai-model-training-internship-in-ahmedabad-at-eonian-software-solutions-private-limited1764090426</t>
+          <t>https://internshala.com/internship/detail/e-commerce-internship-in-bangalore-at-monrow-shoes1764752374</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Innovation Project</t>
+          <t>Client Acquisition</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>STEMpedia</t>
+          <t>SmartED</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore, Andhra Nagar</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>₹ 8,000 - 12,000 /month</t>
+          <t>₹ 26,000 - 28,000 /month</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1391,34 +1391,34 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/innovation-project-internship-in-ahmedabad-at-stempedia1764661414</t>
+          <t>https://internshala.com/internship/detail/client-acquisition-internship-in-multiple-locations-at-smarted1764948248</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Flutter Development</t>
+          <t>Import Export</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Scienext India Private Limited</t>
+          <t>Matrix Exports</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>₹ 7,000 - 12,000 /month</t>
+          <t>₹ 10,000 - 20,000 /month</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1428,34 +1428,34 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/flutter-development-internship-in-multiple-locations-at-scienext-india-private-limited1764582252</t>
+          <t>https://internshala.com/internship/detail/import-export-internship-in-bangalore-at-matrix-exports1764173143</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Computer Operator</t>
+          <t>Media Production</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Multiwa</t>
+          <t>BabyBillion</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>₹ 12,000 - 15,000 /month</t>
+          <t>₹ 10,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1465,34 +1465,34 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/computer-operator-internship-in-ahmedabad-at-multiwa1764948796</t>
+          <t>https://internshala.com/internship/detail/media-production-internship-in-bangalore-at-babybillion1764227906</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>E-Commerce</t>
+          <t>Social Media &amp; Community Engagement</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>The House Of Vraj:bhoomi</t>
+          <t>Prasun Ramdas</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore(Hybrid)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>₹ 8,000 - 15,000 /month</t>
+          <t>₹ 10,000 /month</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1502,34 +1502,34 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/e-commerce-internship-in-ahmedabad-at-the-house-of-vrajbhoomi1764849069</t>
+          <t>https://internshala.com/internship/detail/social-media-community-engagement-internship-in-bangalore-at-prasun-ramdas1764657228</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Internet Of Things (IoT)</t>
+          <t>Telecaller</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Exceliot Technologies Private Limited</t>
+          <t>NutnBolt Business Solution (Dil Foods)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore(Hybrid)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>₹ 5,000 /month</t>
+          <t>₹ 14,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1539,34 +1539,34 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/internet-of-things-iot-internship-in-multiple-locations-at-exceliot-technologies-private-limited1764931430</t>
+          <t>https://internshala.com/internship/detail/telecaller-internship-in-bangalore-at-nutnbolt-business-solution-dil-foods1764756935</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>React Native Development</t>
+          <t>Client Servicing</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Naiplus Solution Private Limited</t>
+          <t>D'ART Private Limited</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>₹ 5,500 - 8,700 /month</t>
+          <t>₹ 25,000 - 35,000 /month</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1576,34 +1576,34 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/react-native-development-internship-in-ahmedabad-at-naiplus-solution-private-limited1765695018</t>
+          <t>https://internshala.com/internship/detail/client-servicing-internship-in-bangalore-at-dart-private-limited1764833595</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>React Native Development</t>
+          <t>Telecalling</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>OrgLance Technologies LLP</t>
+          <t>Enduring Ventures</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>₹ 6,000 - 7,000 /month</t>
+          <t>₹ 12,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1613,34 +1613,34 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/react-native-development-internship-in-ahmedabad-at-orglance-technologies-llp1763555112</t>
+          <t>https://internshala.com/internship/detail/telecalling-internship-in-bangalore-at-enduring-ventures1765355211</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Flutter Development</t>
+          <t>Content Review</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Maxgen Technologies Private Limited</t>
+          <t>Snapmint Credit Advisory Private Limited</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 12,000 /month</t>
+          <t>₹ 5,000 - 8,000 /month</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1650,34 +1650,34 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/flutter-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765353396</t>
+          <t>https://internshala.com/internship/detail/content-review-internship-in-bangalore-at-snapmint-credit-advisory-private-limited1765276303</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Game Development</t>
+          <t>Key Account Associate</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Itechnuts</t>
+          <t>HappyLocate Relocation Services Private Limited</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>₹ 3,000 - 6,000 /month</t>
+          <t>₹ 10,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1687,34 +1687,34 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/game-development-internship-in-ahmedabad-at-itechnuts1765267443</t>
+          <t>https://internshala.com/internship/detail/key-account-associate-internship-in-bangalore-at-happylocate-relocation-services-private-limited1764305737</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Game Development</t>
+          <t>Data Operations Specialist</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
+          <t>Scarlet</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore(Hybrid)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>₹ 30,000 - 40,000 /month</t>
+          <t>₹ 15,000 /month</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1724,34 +1724,34 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/game-development-internship-in-multiple-locations-at-tsteps-private-limited1762153391</t>
+          <t>https://internshala.com/internship/detail/part-time-data-operations-specialist-internship-in-bangalore-at-scarlet1765445980</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Full Stack Development</t>
+          <t>Front Office</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Maxgen Technologies Private Limited</t>
+          <t>UNITED HOSPITAL</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 12,000 /month</t>
+          <t>₹ 5,000 /month</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1761,34 +1761,34 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1764824075</t>
+          <t>https://internshala.com/internship/detail/front-office-internship-in-bangalore-at-united-hospital1765297285</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ReactJS Development</t>
+          <t>Founders Office</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Chaintech Network</t>
+          <t>Finarva</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bellary, Bangalore</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>₹ 9,500 - 10,000 /month</t>
+          <t>₹ 10,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1798,34 +1798,34 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/reactjs-development-internship-in-ahmedabad-at-chaintech-network1764573695</t>
+          <t>https://internshala.com/internship/detail/founders-office-internship-in-multiple-locations-at-fin-tech-startup1765210452</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ReactJS Development</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Maxgen Technologies Private Limited</t>
+          <t>Icecreamlabs</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore(Hybrid)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 12,000 /month</t>
+          <t>₹ 10,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1835,34 +1835,34 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/reactjs-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1764736218</t>
+          <t>https://internshala.com/internship/detail/part-time-marketing-internship-in-bangalore-at-icecreamlabs1762945552</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>SQL Developer</t>
+          <t>Resume with Razorpay - Technical Program Manager</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
+          <t>Razorpay</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>₹ 30,000 - 40,000 /month</t>
+          <t>Competitive stipend</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1872,34 +1872,34 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/sql-developer-internship-in-multiple-locations-at-tsteps-private-limited1762151902</t>
+          <t>https://internshala.com/internship/detail/resume-with-razorpay-technical-program-manager-internship-in-bangalore-at-razorpay1763539890</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>MERN Stack</t>
+          <t>Business Development (Sales)</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Maxgen Technologies Private Limited</t>
+          <t>Saleson Technologies</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 12,000 /month</t>
+          <t>₹ 25,000 /month</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -1909,34 +1909,34 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/part-time-mern-stack-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765357770</t>
+          <t>https://internshala.com/internship/detail/business-development-sales-internship-in-bangalore-at-saleson-technologies1763558853</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Software Testing</t>
+          <t>Train Travel Associate</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
+          <t>Datawise Management Services India Private Limited</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Amritsar, Bhubaneswar, Chennai, Delhi, Guwahati, Indore, Kolkata, Patna, Thiruvananthapuram, Visakhapatnam, Secunderabad, Mumbai, Varanasi, Bangalore, Jammu</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>₹ 30,000 - 40,000 /month</t>
+          <t>₹ 15,000 - 20,000 /month</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1946,34 +1946,34 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/software-testing-internship-in-multiple-locations-at-tsteps-private-limited1762159771</t>
+          <t>https://internshala.com/internship/detail/part-time-train-travel-associate-internship-in-multiple-locations-at-datawise-management-services-india-private-limited1764592085</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Manual Testing</t>
+          <t>E-Commerce</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
+          <t>Cloudnine Hospital</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>₹ 30,000 - 40,000 /month</t>
+          <t>₹ 10,000 /month</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1983,34 +1983,34 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/manual-testing-internship-in-multiple-locations-at-tsteps-private-limited1762157179</t>
+          <t>https://internshala.com/internship/detail/e-commerce-internship-in-bangalore-at-cloudnine-hospital1764645570</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>AI-Machine Lerning</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Maxgen Technologies Private Limited</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 12,000 /month</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2020,34 +2020,34 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/part-time-ai-machine-lerning-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765357926</t>
+          <t>https://internshala.comhttps://internshala.com/internships/work-from-home-data-analyst-internships/?utm_source=wfh_location_message</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Web Development</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Ranogic IT Solutions</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>₹ 3,000 - 6,000 /month</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2057,34 +2057,34 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/web-development-internship-in-ahmedabad-at-ranogic-it-solutions1763112357</t>
+          <t>https://internshala.comhttps://internshala.com/internships/work-from-home-data-analyst-internships/?utm_source=wfh_location_message</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Programming</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>Fresher</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>₹ 30,000 - 40,000 /month</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2094,599 +2094,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/programming-internship-in-multiple-locations-at-tsteps-private-limited1762156258</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Full Stack Development</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Meru Technosoft Private Limited</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Ahmedabad</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>₹ 3,000 - 6,000 /month</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-ahmedabad-at-meru-technosoft-private-limited1763471030</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>PHP Development</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>ECodeSoft Solutions</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Ahmedabad</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>₹ 3,000 - 8,000 /month</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/php-development-internship-in-ahmedabad-at-ecodesoft-solutions1764927058</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>Python Development</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Chaintech Network</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Ahmedabad</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>₹ 9,500 - 10,000 /month</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/python-development-internship-in-ahmedabad-at-chaintech-network1764573338</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>ReactJS Development</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Maxgen Technologies Private Limited</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Ahmedabad</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>₹ 5,000 - 12,000 /month</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/part-time-reactjs-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1764920480</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>JavaScript Development</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Ahmedabad</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>₹ 30,000 - 40,000 /month</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/javascript-development-internship-in-multiple-locations-at-tsteps-private-limited1762158549</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>PHP Development</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Ahmedabad</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>₹ 30,000 - 40,000 /month</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/php-development-internship-in-multiple-locations-at-tsteps-private-limited1762161157</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Full Stack Development</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>WonderBotz</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Ahmedabad</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>₹ 10,000 /month</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-ahmedabad-at-wonderbotz1765800276</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>AWS DevOps Engineer</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Maxgen Technologies Private Limited</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Ahmedabad</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>₹ 5,000 - 12,000 /month</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/aws-devops-engineer-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765603048</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>Flutter Development</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Meru Technosoft Private Limited</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Ahmedabad</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>₹ 3,000 - 5,000 /month</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/flutter-development-internship-in-ahmedabad-at-meru-technosoft-private-limited1765454648</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Quality Analyst</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Ahmedabad</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>₹ 30,000 - 40,000 /month</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/quality-analyst-internship-in-multiple-locations-at-tsteps-private-limited1762161642</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>Embedded Systems</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Ahmedabad</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>₹ 30,000 - 40,000 /month</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/embedded-systems-internship-in-multiple-locations-at-tsteps-private-limited1762156894</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Mobile App Development</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Ahmedabad</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>₹ 30,000 - 40,000 /month</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/mobile-app-development-internship-in-multiple-locations-at-tsteps-private-limited1762159495</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>Web Programmer</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>Maxgen Technologies Private Limited</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Ahmedabad</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>₹ 5,000 - 12,000 /month</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/part-time-web-programmer-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765780187</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>Web Development</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Maxgen Technologies Private Limited</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Ahmedabad</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>₹ 5,000 - 12,000 /month</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/web-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1764577171</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>iOS App Development</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Ahmedabad</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>₹ 30,000 - 40,000 /month</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/ios-app-development-internship-in-multiple-locations-at-tsteps-private-limited1762159806</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>Product Management</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>Coding Junior</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Ahmedabad</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>₹ 15,000 /month</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/product-management-internship-in-multiple-locations-at-coding-junior1764562748</t>
+          <t>https://internshala.comhttps://internshala.com/internships/work-from-home-data-analyst-internships/?utm_source=wfh_location_message</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance job entry display by including job descriptions and improving DataFrame formatting
</commit_message>
<xml_diff>
--- a/output/jobs.xlsx
+++ b/output/jobs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,1650 +451,3205 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Experience</t>
+          <t>Experience Required</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Salary</t>
+          <t>Salary / Stipend</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Posted Date</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Job Portal</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Job URL</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Skills / Role</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Duration</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>College Intern</t>
+          <t>Ecodesoft solutions</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hewlett Packard</t>
+          <t>Ecodesoft solutions</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Competitive stipend</t>
+          <t>3000 - 10000 Monthly</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>7 days ago</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/college-intern-internship-in-bangalore-at-hewlett-packard1758536943</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Operations And Strategy</t>
+          <t>Ecodesoft solutions</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>EkStep</t>
+          <t>Ecodesoft solutions</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>₹ 15,000 - 20,000 /month</t>
+          <t>3000 - 10000 Monthly</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>7 days ago</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/operations-and-strategy-internship-in-bangalore-at-ekstep1762504606</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Business Development Intern</t>
+          <t>Devine Globe Technologies</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>PlatinumRx.in</t>
+          <t>Devine Globe Technologies</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>2 to 3 Years</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>₹ 15,000 - 25,000 /month</t>
+          <t>20000 - 35000 Monthly</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>14 days ago</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/partnership-internship-in-bangalore-at-platinumrxin1763702380</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Technical Writer</t>
+          <t>RB HR Solutions</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DTALES Tech</t>
+          <t>RB HR Solutions</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Bangalore(Hybrid)</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>3+ Years</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>₹ 15,000 /month</t>
+          <t>58000 - 100000 Monthly</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/technical-writer-internship-in-bangalore-at-dtales-tech1764236817</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Digital Marketing</t>
+          <t>Hamilton Services</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Chola Apparels</t>
+          <t>Hamilton Services</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>1 to 3 Years</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 8,000 /month</t>
+          <t>5000 - 50000 Monthly</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/digital-marketing-internship-in-bangalore-at-chola-apparels1764163866</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Supply Chain Management (SCM)</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Monrow Shoes</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>₹ 15,000 /month</t>
+          <t>Salary not disclosed</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/supply-chain-management-scm-internship-in-bangalore-at-monrow-shoes1764226109</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Data Entry</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>NoBroker</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>₹ 12,000 - 15,000 /month</t>
+          <t>Salary not disclosed</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/data-entry-internship-in-bangalore-at-nobroker1764254680</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Technical Program Manager</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Razorpay</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>3+ Years</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Competitive stipend</t>
+          <t>Salary not disclosed</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/technical-program-manager-internship-in-bangalore-at-razorpay1764311275</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Content and Social Media Marketing</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Fiscal Flow</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>₹ 8,000 - 14,000 /month</t>
+          <t>Salary not disclosed</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/content-and-social-media-marketing-internship-in-bangalore-at-fiscal-flow1763467186</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Founders Office &amp; Marketing</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SuperU</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>₹ 15,000 - 30,000 /month</t>
+          <t>Salary not disclosed</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/founders-office-marketing-internship-in-bangalore-at-superu1763461248</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>⭐ 4.5</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Salary not disclosed</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Community Activation</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Marzi By Primus</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>₹ 15,000 - 20,000 /month</t>
+          <t>Salary not disclosed</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/community-activation-internship-in-bangalore-at-marzi-by-primus1763551901</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Marketing Research &amp; Analytics</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CertPro</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>₹ 15,000 - 25,000 /month</t>
+          <t>Salary not disclosed</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/marketing-research-analytics-internship-in-bangalore-at-certpro1763608097</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Customer Service/Customer Support</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>AQ Corporation India Private Limited</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>₹ 7,500 - 10,000 /month</t>
+          <t>Salary not disclosed</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/customer-service-customer-support-internship-in-bangalore-at-aq-corporation-india-private-limited1763556900</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>E-Commerce Operations</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>RuralEquip PVT Ltd</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>₹ 8,000 - 15,000 /month</t>
+          <t>Salary not disclosed</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/e-commerce-operations-internship-in-bangalore-at-ruralequip-pvt-ltd1764168724</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Content and Social Media Marketing</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Tanai Balaji</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Bangalore(Hybrid)</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>₹ 4,000 - 6,000 /month</t>
+          <t>Salary not disclosed</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/part-time-content-and-social-media-marketing-internship-in-bangalore-at-tanai-balaji1764226392</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Customer Service/Customer Support</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Sugar.fit</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>₹ 15,000 /month</t>
+          <t>Salary not disclosed</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/customer-service-customer-support-internship-in-bangalore-at-sugarfit1764219786</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Key Account Associate</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>HappyLocate Relocation Services Private Limited</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>₹ 10,000 - 15,000 /month</t>
+          <t>Salary not disclosed</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/key-account-associate-internship-in-bangalore-at-happylocate-relocation-services-private-limited1764238570</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Telecalling</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Infocruise Solutions Private LImited</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>2 to 3+ Years</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>₹ 8,500 - 10,000 /month</t>
+          <t>Salary not disclosed</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/telecalling-internship-in-bangalore-at-infocruise-solutions-private-limited1764241856</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Event Management</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>NYUC Technologies</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Delhi, Hyderabad, Mumbai, Bangalore(Hybrid)</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>₹ 15,000 /month</t>
+          <t>Salary not disclosed</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/event-management-internship-in-multiple-locations-at-nyuc-technologies1763959180</t>
-        </is>
-      </c>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Client Servicing</t>
+          <t>Internet Of Things (IoT)</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>WILDFOX BUSINESS ADVOCACY</t>
+          <t>Exceliot Technologies Private Limited</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad, Gandhinagar</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>₹ 2,000 /month</t>
+          <t>₹ 5,000 /month</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 week ago</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/client-servicing-internship-in-bangalore-at-wildfox-business-advocacy1764689795</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/internet-of-things-iot-internship-in-multiple-locations-at-exceliot-technologies-private-limited1764931430</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>GTM</t>
+          <t>Information Technology</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>FirstClub Technology Private Limited</t>
+          <t>ITGS Infotech Private Limited</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad, Bhubaneswar, Chandigarh, Chennai, Indore, Kolkata, Lucknow, Hyderabad, Mumbai, Kochi, Jaipur, Bangalore(Hybrid)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>₹ 25,000 - 30,000 /month</t>
+          <t>₹ 10,000 - 20,000 /month</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/gtm-internship-in-bangalore-at-firstclub-technology-private-limited1764829004</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/part-time-information-technology-internship-in-multiple-locations-at-itgs-infotech-private-limited1764671132</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Office Assistant</t>
+          <t>Computer Operator</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Shree Impex</t>
+          <t>Multiwa</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Bangalore, Koramangala</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>₹ 2,000 - 7,000 /month</t>
+          <t>₹ 12,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 week ago</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/office-assistant-internship-in-multiple-locations-at-shree-impex1763461455</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/computer-operator-internship-in-ahmedabad-at-multiwa1764948796</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>E-Commerce</t>
+          <t>iOS App Development</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Monrow Shoes</t>
+          <t>TSTEPS PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Chennai, Mumbai, Bangalore, Kerala, Puduchery, Karnataka(Hybrid)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>₹ 15,000 /month</t>
+          <t>₹ 30,000 - 40,000 /month</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/e-commerce-internship-in-bangalore-at-monrow-shoes1764752374</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/ios-app-development-internship-in-multiple-locations-at-tsteps-private-limited1762159806</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Client Acquisition</t>
+          <t>Flutter Development</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SmartED</t>
+          <t>Scienext India Private Limited</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bangalore, Andhra Nagar</t>
+          <t>Ahmedabad, Gandhinagar</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>₹ 26,000 - 28,000 /month</t>
+          <t>₹ 7,000 - 12,000 /month</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/client-acquisition-internship-in-multiple-locations-at-smarted1764948248</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/flutter-development-internship-in-multiple-locations-at-scienext-india-private-limited1764582252</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Import Export</t>
+          <t>React Native Development</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Matrix Exports</t>
+          <t>Naiplus Solution Private Limited</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>₹ 10,000 - 20,000 /month</t>
+          <t>₹ 5,500 - 8,700 /month</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>4 days ago</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/import-export-internship-in-bangalore-at-matrix-exports1764173143</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/react-native-development-internship-in-ahmedabad-at-naiplus-solution-private-limited1765695018</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Media Production</t>
+          <t>Flutter Development</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BabyBillion</t>
+          <t>Meru Technosoft Private Limited</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>₹ 10,000 - 15,000 /month</t>
+          <t>₹ 3,000 - 5,000 /month</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>7 days ago</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/media-production-internship-in-bangalore-at-babybillion1764227906</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/flutter-development-internship-in-ahmedabad-at-meru-technosoft-private-limited1765454648</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Social Media &amp; Community Engagement</t>
+          <t>PHP Development</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Prasun Ramdas</t>
+          <t>TSTEPS PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Bangalore(Hybrid)</t>
+          <t>Chennai, Hyderabad, Kerala, Mumbai, Karnataka(Hybrid)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>₹ 10,000 /month</t>
+          <t>₹ 30,000 - 40,000 /month</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/social-media-community-engagement-internship-in-bangalore-at-prasun-ramdas1764657228</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/php-development-internship-in-multiple-locations-at-tsteps-private-limited1762161157</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Telecaller</t>
+          <t>Web Development</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>NutnBolt Business Solution (Dil Foods)</t>
+          <t>Ranogic IT Solutions</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Bangalore(Hybrid)</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>₹ 14,000 - 15,000 /month</t>
+          <t>₹ 3,000 - 6,000 /month</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/telecaller-internship-in-bangalore-at-nutnbolt-business-solution-dil-foods1764756935</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/web-development-internship-in-ahmedabad-at-ranogic-it-solutions1763112357</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Client Servicing</t>
+          <t>Internet Of Things (IoT)</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>D'ART Private Limited</t>
+          <t>DIPC Tech Private Limited</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>₹ 25,000 - 35,000 /month</t>
+          <t>₹ 6,000 - 11,000 /month</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/client-servicing-internship-in-bangalore-at-dart-private-limited1764833595</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/internet-of-things-iot-internship-in-ahmedabad-at-dipc-tech-private-limited1763616274</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Telecalling</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Enduring Ventures</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>₹ 12,000 - 15,000 /month</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>Recently Posted</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/telecalling-internship-in-bangalore-at-enduring-ventures1765355211</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Content Review</t>
+          <t>SQL Developer</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Snapmint Credit Advisory Private Limited</t>
+          <t>TSTEPS PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Chennai, Mumbai, Hyderabad, Kerala, Karnataka(Hybrid)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 8,000 /month</t>
+          <t>₹ 30,000 - 40,000 /month</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/content-review-internship-in-bangalore-at-snapmint-credit-advisory-private-limited1765276303</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/sql-developer-internship-in-multiple-locations-at-tsteps-private-limited1762151902</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Key Account Associate</t>
+          <t>Manual Testing</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>HappyLocate Relocation Services Private Limited</t>
+          <t>TSTEPS PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Chennai, Mumbai, Bangalore, Kerala, Karnataka(Hybrid)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>₹ 10,000 - 15,000 /month</t>
+          <t>₹ 30,000 - 40,000 /month</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/key-account-associate-internship-in-bangalore-at-happylocate-relocation-services-private-limited1764305737</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/manual-testing-internship-in-multiple-locations-at-tsteps-private-limited1762157179</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Data Operations Specialist</t>
+          <t>React Native Development</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Scarlet</t>
+          <t>OrgLance Technologies LLP</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Bangalore(Hybrid)</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>₹ 15,000 /month</t>
+          <t>₹ 6,000 - 7,000 /month</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/part-time-data-operations-specialist-internship-in-bangalore-at-scarlet1765445980</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/react-native-development-internship-in-ahmedabad-at-orglance-technologies-llp1763555112</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Front Office</t>
+          <t>Mobile App Development</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>UNITED HOSPITAL</t>
+          <t>Rechain Technologies Private Limited</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>₹ 5,000 /month</t>
+          <t>₹ 5,000 - 30,000 /month</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>Today</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/front-office-internship-in-bangalore-at-united-hospital1765297285</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/mobile-app-development-internship-in-ahmedabad-at-rechain-technologies-private-limited1765990832</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Founders Office</t>
+          <t>AI-Machine Lerning</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Finarva</t>
+          <t>Maxgen Technologies Private Limited</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Bellary, Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>₹ 10,000 - 15,000 /month</t>
+          <t>₹ 5,000 - 12,000 /month</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 week ago</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/founders-office-internship-in-multiple-locations-at-fin-tech-startup1765210452</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/part-time-ai-machine-lerning-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765357926</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Game Development</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Icecreamlabs</t>
+          <t>Itechnuts</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Bangalore(Hybrid)</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>₹ 10,000 - 15,000 /month</t>
+          <t>₹ 3,000 - 6,000 /month</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 week ago</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/part-time-marketing-internship-in-bangalore-at-icecreamlabs1762945552</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/game-development-internship-in-ahmedabad-at-itechnuts1765267443</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Resume with Razorpay - Technical Program Manager</t>
+          <t>Innovation Project</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Razorpay</t>
+          <t>STEMpedia</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Competitive stipend</t>
+          <t>₹ 8,000 - 12,000 /month</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/resume-with-razorpay-technical-program-manager-internship-in-bangalore-at-razorpay1763539890</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/innovation-project-internship-in-ahmedabad-at-stempedia1764661414</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Business Development (Sales)</t>
+          <t>E-Commerce</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Saleson Technologies</t>
+          <t>The House Of Vraj:bhoomi</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>₹ 25,000 /month</t>
+          <t>₹ 8,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/business-development-sales-internship-in-bangalore-at-saleson-technologies1763558853</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/e-commerce-internship-in-ahmedabad-at-the-house-of-vrajbhoomi1764849069</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Train Travel Associate</t>
+          <t>Data Annotations For AI Model Training</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Datawise Management Services India Private Limited</t>
+          <t>Eonian Software Solutions Private Limited</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Amritsar, Bhubaneswar, Chennai, Delhi, Guwahati, Indore, Kolkata, Patna, Thiruvananthapuram, Visakhapatnam, Secunderabad, Mumbai, Varanasi, Bangalore, Jammu</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>₹ 15,000 - 20,000 /month</t>
+          <t>₹ 2,500 - 4,000 /month</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/part-time-train-travel-associate-internship-in-multiple-locations-at-datawise-management-services-india-private-limited1764592085</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/part-time-data-annotations-for-ai-model-training-internship-in-ahmedabad-at-eonian-software-solutions-private-limited1764090426</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>E-Commerce</t>
+          <t>PHP Development</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Cloudnine Hospital</t>
+          <t>ECodeSoft Solutions</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>₹ 10,000 /month</t>
+          <t>₹ 3,000 - 8,000 /month</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 week ago</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/e-commerce-internship-in-bangalore-at-cloudnine-hospital1764645570</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/php-development-internship-in-ahmedabad-at-ecodesoft-solutions1764927058</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Flutter Development</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Maxgen Technologies Private Limited</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Banglore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>₹ 5,000 - 12,000 /month</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 week ago</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://internshala.comhttps://internshala.com/internships/work-from-home-data-analyst-internships/?utm_source=wfh_location_message</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/flutter-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765353396</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>MERN Stack</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Maxgen Technologies Private Limited</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Banglore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>₹ 5,000 - 12,000 /month</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>1 week ago</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://internshala.comhttps://internshala.com/internships/work-from-home-data-analyst-internships/?utm_source=wfh_location_message</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/part-time-mern-stack-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765357770</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Web Development</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Maxgen Technologies Private Limited</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Banglore</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>₹ 5,000 - 12,000 /month</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Internshala</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://internshala.comhttps://internshala.com/internships/work-from-home-data-analyst-internships/?utm_source=wfh_location_message</t>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/web-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1764577171</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Full Stack Development</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Maxgen Technologies Private Limited</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Ahmedabad</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>₹ 5,000 - 12,000 /month</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2 weeks ago</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1764824075</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Web Programmer</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Maxgen Technologies Private Limited</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Ahmedabad</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>₹ 5,000 - 12,000 /month</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>3 days ago</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/part-time-web-programmer-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765780187</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Quality Analyst</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>TSTEPS PRIVATE LIMITED</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Chennai, Mumbai, Bangalore, Kerala, Puduchery(Hybrid)</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>₹ 30,000 - 40,000 /month</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/quality-analyst-internship-in-multiple-locations-at-tsteps-private-limited1762161642</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Mobile App Development</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>TSTEPS PRIVATE LIMITED</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Chennai, Mumbai, Hyderabad, Bangalore, Kerala, Puduchery(Hybrid)</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>₹ 30,000 - 40,000 /month</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/mobile-app-development-internship-in-multiple-locations-at-tsteps-private-limited1762159495</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Full Stack Development</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>WonderBotz</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Ahmedabad</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>₹ 10,000 /month</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>3 days ago</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-ahmedabad-at-wonderbotz1765800276</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Full Stack Development</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Meru Technosoft Private Limited</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Ahmedabad</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>₹ 3,000 - 6,000 /month</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-ahmedabad-at-meru-technosoft-private-limited1763471030</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Product Management</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Coding Junior</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Ahmedabad, Bhubaneswar, Delhi, Surat, Hyderabad, Bhopal, Mumbai, Jaipur</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>₹ 15,000 /month</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2 weeks ago</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/product-management-internship-in-multiple-locations-at-coding-junior1764562748</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>ReactJS Development</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Chaintech Network</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Ahmedabad</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>₹ 9,500 - 10,000 /month</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>2 weeks ago</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/reactjs-development-internship-in-ahmedabad-at-chaintech-network1764573695</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>JavaScript Development</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>TSTEPS PRIVATE LIMITED</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Chennai, Coimbatore, Mumbai, Bangalore, Kerala(Hybrid)</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>₹ 30,000 - 40,000 /month</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/javascript-development-internship-in-multiple-locations-at-tsteps-private-limited1762158549</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Game Development</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>TSTEPS PRIVATE LIMITED</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Chennai, Hyderabad, Mumbai, Kerala(Hybrid)</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>₹ 30,000 - 40,000 /month</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/game-development-internship-in-multiple-locations-at-tsteps-private-limited1762153391</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Software Testing</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>TSTEPS PRIVATE LIMITED</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Chennai, Coimbatore, Mumbai, Hyderabad, Kerala(Hybrid)</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>₹ 30,000 - 40,000 /month</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/software-testing-internship-in-multiple-locations-at-tsteps-private-limited1762159771</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Programming</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>TSTEPS PRIVATE LIMITED</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Chennai, Coimbatore, Mumbai, Bangalore, Kerala(Hybrid)</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>₹ 30,000 - 40,000 /month</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/programming-internship-in-multiple-locations-at-tsteps-private-limited1762156258</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>ReactJS Development</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Maxgen Technologies Private Limited</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Ahmedabad</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>₹ 5,000 - 12,000 /month</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>2 weeks ago</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/reactjs-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1764736218</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>ReactJS Development</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Maxgen Technologies Private Limited</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Ahmedabad</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>₹ 5,000 - 12,000 /month</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>1 week ago</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/part-time-reactjs-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1764920480</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Data Anlayst</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Maxgen Technologies Private Limited</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Ahmedabad</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>₹ 5,000 - 12,000 /month</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>1 week ago</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/part-time-data-anlayst-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765003178</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Embedded Systems</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>TSTEPS PRIVATE LIMITED</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Chennai, Mumbai, Hyderabad, Bangalore, Kerala(Hybrid)</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>₹ 30,000 - 40,000 /month</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/embedded-systems-internship-in-multiple-locations-at-tsteps-private-limited1762156894</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>AR/VR</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>AgroCast Analytics Private Limited</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Gandhinagar</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>₹ 5,000 - 7,000 /month</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/ar-vr-internship-in-gandhinagar-at-agrocast-analytics-private-limited1763559663</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Ahmedabad</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Recently Posted</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internships/work-from-home-python-developer-internships/?utm_source=wfh_location_message</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Ahmedabad</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Recently Posted</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internships/work-from-home-python-developer-internships/?utm_source=wfh_location_message</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Ahmedabad</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Recently Posted</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internships/work-from-home-python-developer-internships/?utm_source=wfh_location_message</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve job data export by adding support for CSV format and optimizing data retrieval process
</commit_message>
<xml_diff>
--- a/output/jobs.xlsx
+++ b/output/jobs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,10 +476,15 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>Searched Job Title</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Skills / Role</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Duration</t>
         </is>
@@ -526,8 +531,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -570,8 +580,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -614,8 +629,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -658,8 +678,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -702,8 +727,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -746,8 +776,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -790,8 +825,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -834,8 +874,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -878,8 +923,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -922,8 +972,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -966,8 +1021,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1010,8 +1070,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1054,8 +1119,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1098,8 +1168,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1142,8 +1217,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1186,8 +1266,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1230,8 +1315,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1274,8 +1364,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1318,8 +1413,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1362,8 +1462,13 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Python Developer</t>
+        </is>
+      </c>
       <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1408,10 +1513,15 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1460,10 +1570,15 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1512,10 +1627,15 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1564,10 +1684,15 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1616,10 +1741,15 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1668,10 +1798,15 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1720,10 +1855,15 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1772,10 +1912,15 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1824,10 +1969,15 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1876,10 +2026,15 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1928,10 +2083,15 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1980,10 +2140,15 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2032,10 +2197,15 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2084,10 +2254,15 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2136,10 +2311,15 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2188,10 +2368,15 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2240,10 +2425,15 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2292,10 +2482,15 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2344,10 +2539,15 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2396,10 +2596,15 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2408,12 +2613,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>PHP Development</t>
+          <t>Flutter Development</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ECodeSoft Solutions</t>
+          <t>Maxgen Technologies Private Limited</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2428,7 +2633,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>₹ 3,000 - 8,000 /month</t>
+          <t>₹ 5,000 - 12,000 /month</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2443,15 +2648,20 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/php-development-internship-in-ahmedabad-at-ecodesoft-solutions1764927058</t>
+          <t>https://internshala.com/internship/detail/flutter-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765353396</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2460,7 +2670,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Flutter Development</t>
+          <t>MERN Stack</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2495,15 +2705,20 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/flutter-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765353396</t>
+          <t>https://internshala.com/internship/detail/part-time-mern-stack-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765357770</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2512,7 +2727,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>MERN Stack</t>
+          <t>Web Development</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2537,7 +2752,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>1 week ago</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -2547,15 +2762,20 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/part-time-mern-stack-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765357770</t>
+          <t>https://internshala.com/internship/detail/web-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1764577171</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2564,7 +2784,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Web Development</t>
+          <t>Full Stack Development</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2599,15 +2819,20 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/web-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1764577171</t>
+          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1764824075</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2616,7 +2841,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Full Stack Development</t>
+          <t>Web Programmer</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2641,7 +2866,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2 weeks ago</t>
+          <t>3 days ago</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -2651,15 +2876,20 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1764824075</t>
+          <t>https://internshala.com/internship/detail/part-time-web-programmer-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765780187</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2668,17 +2898,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Web Programmer</t>
+          <t>Quality Analyst</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Maxgen Technologies Private Limited</t>
+          <t>TSTEPS PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Chennai, Mumbai, Bangalore, Kerala, Puduchery(Hybrid)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2688,12 +2918,12 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 12,000 /month</t>
+          <t>₹ 30,000 - 40,000 /month</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>3 days ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2703,15 +2933,20 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/part-time-web-programmer-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765780187</t>
+          <t>https://internshala.com/internship/detail/quality-analyst-internship-in-multiple-locations-at-tsteps-private-limited1762161642</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2720,7 +2955,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Quality Analyst</t>
+          <t>Mobile App Development</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2730,7 +2965,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Chennai, Mumbai, Bangalore, Kerala, Puduchery(Hybrid)</t>
+          <t>Chennai, Mumbai, Hyderabad, Bangalore, Kerala, Puduchery(Hybrid)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2755,15 +2990,20 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/quality-analyst-internship-in-multiple-locations-at-tsteps-private-limited1762161642</t>
+          <t>https://internshala.com/internship/detail/mobile-app-development-internship-in-multiple-locations-at-tsteps-private-limited1762159495</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2772,17 +3012,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Mobile App Development</t>
+          <t>Full Stack Development</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
+          <t>WonderBotz</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Chennai, Mumbai, Hyderabad, Bangalore, Kerala, Puduchery(Hybrid)</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2792,12 +3032,12 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>₹ 30,000 - 40,000 /month</t>
+          <t>₹ 10,000 /month</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>3 days ago</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -2807,15 +3047,20 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/mobile-app-development-internship-in-multiple-locations-at-tsteps-private-limited1762159495</t>
+          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-ahmedabad-at-wonderbotz1765800276</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2829,7 +3074,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>WonderBotz</t>
+          <t>Meru Technosoft Private Limited</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2844,12 +3089,12 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>₹ 10,000 /month</t>
+          <t>₹ 3,000 - 6,000 /month</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>3 days ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -2859,15 +3104,20 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-ahmedabad-at-wonderbotz1765800276</t>
+          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-ahmedabad-at-meru-technosoft-private-limited1763471030</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2876,17 +3126,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Full Stack Development</t>
+          <t>Product Management</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Meru Technosoft Private Limited</t>
+          <t>Coding Junior</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Ahmedabad, Bhubaneswar, Delhi, Surat, Hyderabad, Bhopal, Mumbai, Jaipur</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2896,12 +3146,12 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>₹ 3,000 - 6,000 /month</t>
+          <t>₹ 15,000 /month</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2911,15 +3161,20 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-ahmedabad-at-meru-technosoft-private-limited1763471030</t>
+          <t>https://internshala.com/internship/detail/product-management-internship-in-multiple-locations-at-coding-junior1764562748</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2928,17 +3183,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Product Management</t>
+          <t>ReactJS Development</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Coding Junior</t>
+          <t>Chaintech Network</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Ahmedabad, Bhubaneswar, Delhi, Surat, Hyderabad, Bhopal, Mumbai, Jaipur</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2948,7 +3203,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>₹ 15,000 /month</t>
+          <t>₹ 9,500 - 10,000 /month</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2963,15 +3218,20 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/product-management-internship-in-multiple-locations-at-coding-junior1764562748</t>
+          <t>https://internshala.com/internship/detail/reactjs-development-internship-in-ahmedabad-at-chaintech-network1764573695</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2980,17 +3240,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>ReactJS Development</t>
+          <t>Programming</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Chaintech Network</t>
+          <t>TSTEPS PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Chennai, Coimbatore, Mumbai, Bangalore, Kerala(Hybrid)</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -3000,12 +3260,12 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>₹ 9,500 - 10,000 /month</t>
+          <t>₹ 30,000 - 40,000 /month</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2 weeks ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -3015,15 +3275,20 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/reactjs-development-internship-in-ahmedabad-at-chaintech-network1764573695</t>
+          <t>https://internshala.com/internship/detail/programming-internship-in-multiple-locations-at-tsteps-private-limited1762156258</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3032,17 +3297,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>JavaScript Development</t>
+          <t>ReactJS Development</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
+          <t>Maxgen Technologies Private Limited</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Chennai, Coimbatore, Mumbai, Bangalore, Kerala(Hybrid)</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -3052,12 +3317,12 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>₹ 30,000 - 40,000 /month</t>
+          <t>₹ 5,000 - 12,000 /month</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -3067,15 +3332,20 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/javascript-development-internship-in-multiple-locations-at-tsteps-private-limited1762158549</t>
+          <t>https://internshala.com/internship/detail/reactjs-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1764736218</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3084,17 +3354,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Game Development</t>
+          <t>ReactJS Development</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
+          <t>Maxgen Technologies Private Limited</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Chennai, Hyderabad, Mumbai, Kerala(Hybrid)</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -3104,12 +3374,12 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>₹ 30,000 - 40,000 /month</t>
+          <t>₹ 5,000 - 12,000 /month</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>1 week ago</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -3119,15 +3389,20 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/game-development-internship-in-multiple-locations-at-tsteps-private-limited1762153391</t>
+          <t>https://internshala.com/internship/detail/part-time-reactjs-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1764920480</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3136,17 +3411,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Software Testing</t>
+          <t>Data Anlayst</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
+          <t>Maxgen Technologies Private Limited</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Chennai, Coimbatore, Mumbai, Hyderabad, Kerala(Hybrid)</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -3156,12 +3431,12 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>₹ 30,000 - 40,000 /month</t>
+          <t>₹ 5,000 - 12,000 /month</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>1 week ago</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -3171,15 +3446,20 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/software-testing-internship-in-multiple-locations-at-tsteps-private-limited1762159771</t>
+          <t>https://internshala.com/internship/detail/part-time-data-anlayst-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765003178</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3188,7 +3468,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Programming</t>
+          <t>Embedded Systems</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -3198,7 +3478,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Chennai, Coimbatore, Mumbai, Bangalore, Kerala(Hybrid)</t>
+          <t>Chennai, Mumbai, Hyderabad, Bangalore, Kerala(Hybrid)</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -3223,15 +3503,20 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/programming-internship-in-multiple-locations-at-tsteps-private-limited1762156258</t>
+          <t>https://internshala.com/internship/detail/embedded-systems-internship-in-multiple-locations-at-tsteps-private-limited1762156894</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3240,17 +3525,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>ReactJS Development</t>
+          <t>JavaScript Development</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Maxgen Technologies Private Limited</t>
+          <t>TSTEPS PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Chennai, Coimbatore, Mumbai, Bangalore, Kerala(Hybrid)</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -3260,12 +3545,12 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 12,000 /month</t>
+          <t>₹ 30,000 - 40,000 /month</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2 weeks ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -3275,15 +3560,20 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/reactjs-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1764736218</t>
+          <t>https://internshala.com/internship/detail/javascript-development-internship-in-multiple-locations-at-tsteps-private-limited1762158549</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3292,17 +3582,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>ReactJS Development</t>
+          <t>Game Development</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Maxgen Technologies Private Limited</t>
+          <t>TSTEPS PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Chennai, Hyderabad, Mumbai, Kerala(Hybrid)</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -3312,12 +3602,12 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 12,000 /month</t>
+          <t>₹ 30,000 - 40,000 /month</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>1 week ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -3327,15 +3617,20 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/part-time-reactjs-development-internship-in-ahmedabad-at-maxgen-technologies-private-limited1764920480</t>
+          <t>https://internshala.com/internship/detail/game-development-internship-in-multiple-locations-at-tsteps-private-limited1762153391</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3344,17 +3639,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Data Anlayst</t>
+          <t>Software Testing</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Maxgen Technologies Private Limited</t>
+          <t>TSTEPS PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Chennai, Coimbatore, Mumbai, Hyderabad, Kerala(Hybrid)</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -3364,12 +3659,12 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 12,000 /month</t>
+          <t>₹ 30,000 - 40,000 /month</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>1 week ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -3379,15 +3674,20 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/part-time-data-anlayst-internship-in-ahmedabad-at-maxgen-technologies-private-limited1765003178</t>
+          <t>https://internshala.com/internship/detail/software-testing-internship-in-multiple-locations-at-tsteps-private-limited1762159771</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3396,17 +3696,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Embedded Systems</t>
+          <t>PHP Development</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
+          <t>ECodeSoft Solutions</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Chennai, Mumbai, Hyderabad, Bangalore, Kerala(Hybrid)</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -3416,12 +3716,12 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>₹ 30,000 - 40,000 /month</t>
+          <t>₹ 3,000 - 8,000 /month</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>1 week ago</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -3431,15 +3731,20 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/embedded-systems-internship-in-multiple-locations-at-tsteps-private-limited1762156894</t>
+          <t>https://internshala.com/internship/detail/php-development-internship-in-ahmedabad-at-ecodesoft-solutions1764927058</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3488,10 +3793,15 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3540,10 +3850,15 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3592,10 +3907,15 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3644,10 +3964,15 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>

</xml_diff>

<commit_message>
Refactor job search results processing to streamline data handling and improve display of job details, including enhanced formatting for better readability.
</commit_message>
<xml_diff>
--- a/output/jobs.xlsx
+++ b/output/jobs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,20 +461,30 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Skills / Role</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Duration</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Posted Date</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Job Portal</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Job URL</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Searched Job Title</t>
         </is>
@@ -483,17 +493,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>TECHSHELL SOFTWARE PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>TECHSHELL SOFTWARE PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -503,25 +513,35 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Salary not disclosed</t>
+          <t>240000 - 400000 Yearly</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1 months ago</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>1 days ago</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>Freshersworld</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>Web Developer</t>
         </is>
@@ -530,45 +550,55 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>ServiceNow Software Development India Pvt .Ltd</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>ServiceNow Software Development India Pvt .Ltd</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0 Years</t>
+          <t>3 to 7 Years</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Salary not disclosed</t>
+          <t>500000 - 900000 Yearly</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1 months ago</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>10 days ago</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>Freshersworld</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>Web Developer</t>
         </is>
@@ -577,45 +607,55 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>One Vision Study Abroad</t>
+          <t>Accenture Solutions Pvt Ltd</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>One Vision Study Abroad</t>
+          <t>Accenture Solutions Pvt Ltd</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0 to 0.6 Years</t>
+          <t>4 to 10 Years</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2000 - 5000 Monthly</t>
+          <t>200000 - 700000 Monthly</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1 months ago</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>12 days ago</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
           <t>Freshersworld</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>Web Developer</t>
         </is>
@@ -624,45 +664,55 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>For a Client of TeamLease Digital</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>For a Client of TeamLease Digital</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0 Years</t>
+          <t>2 to 3 Years</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Salary not disclosed</t>
+          <t>300000 - 600000 Yearly</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1 months ago</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>22 days ago</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
           <t>Freshersworld</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>Web Developer</t>
         </is>
@@ -671,17 +721,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>Biogen Capability Center India Private limited</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>Biogen Capability Center India Private limited</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -691,25 +741,35 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Salary not disclosed</t>
+          <t>200000 - 2500000 Monthly</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>1 months ago</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>3 months ago</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
           <t>Freshersworld</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>Web Developer</t>
         </is>
@@ -718,17 +778,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>NITI TECHNOLOGIES INDIA SOFTWARE</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>NITI TECHNOLOGIES INDIA SOFTWARE</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -738,25 +798,35 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Salary not disclosed</t>
+          <t>18500 - 85200 Monthly</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1 months ago</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>1 days ago</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
           <t>Freshersworld</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>Web Developer</t>
         </is>
@@ -765,45 +835,55 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>Ray Business Technologies Pvt Ltd</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>Ray Business Technologies Pvt Ltd</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0 Years</t>
+          <t>0 to 0.6 Years</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Salary not disclosed</t>
+          <t>15000 - 16000 Monthly</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>1 months ago</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2 days ago</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
           <t>Freshersworld</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>Web Developer</t>
         </is>
@@ -812,45 +892,55 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>Mphasis</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>Mphasis</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3+ Years</t>
+          <t>3 Years</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Salary not disclosed</t>
+          <t>120000 - 140000 Monthly</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>1 months ago</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>6 days ago</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
           <t>Freshersworld</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>Web Developer</t>
         </is>
@@ -859,45 +949,55 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>Innasoft Techonologies</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>Innasoft Techonologies</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0 Years</t>
+          <t>2 to 2.5 Years</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Salary not disclosed</t>
+          <t>20000 - 50000 Monthly</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
           <t>1 months ago</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>Freshersworld</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>Web Developer</t>
         </is>
@@ -906,45 +1006,55 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>Digital Jockey</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>Digital Jockey</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0 Years</t>
+          <t>2 to 3+ Years</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Salary not disclosed</t>
+          <t>15000 - 25000 Monthly</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
           <t>1 months ago</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>Freshersworld</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>Web Developer</t>
         </is>
@@ -953,45 +1063,55 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>Apex Web Services</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>Apex Web Services</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0 Years</t>
+          <t>0.6 to 1.5 Years</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Salary not disclosed</t>
+          <t>10000 - 35000 Monthly</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
           <t>1 months ago</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>Freshersworld</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>Web Developer</t>
         </is>
@@ -1000,12 +1120,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Accenture Solutions Pvt Ltd</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Accenture Solutions Pvt Ltd</t>
+          <t>A Client of Freshersworld</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1020,401 +1140,35 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>200000 - 400000 Monthly</t>
+          <t>Salary not disclosed</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>28 days ago</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>1 months ago</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
           <t>Freshersworld</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Accenture Solutions Pvt Ltd</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Accenture Solutions Pvt Ltd</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Hyderabad</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>4 to 10 Years</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>200000 - 500000 Monthly</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>1 months ago</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Freshersworld</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>A Client of Freshersworld</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>A Client of Freshersworld</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Delhi</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>0 Years</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Salary not disclosed</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>1 months ago</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Freshersworld</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>A client of Freshersworld</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>A client of Freshersworld</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Delhi</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>0 Years</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Salary not disclosed</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>1 months ago</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Freshersworld</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>A Client of Freshersworld</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>A Client of Freshersworld</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Delhi</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>0 Years</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Salary not disclosed</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2 months ago</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Freshersworld</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>A Client of Freshersworld</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>A Client of Freshersworld</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Delhi</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>0 Years</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Salary not disclosed</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>1 months ago</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Freshersworld</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>A Client of Freshersworld</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>A Client of Freshersworld</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Delhi</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>0 Years</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Salary not disclosed</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>1 months ago</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Freshersworld</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>A Client of Freshersworld</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>A Client of Freshersworld</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Delhi</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>0 Years</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Salary not disclosed</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>1 months ago</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Freshersworld</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>A Client of Freshersworld</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>A Client of Freshersworld</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Delhi</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>0 Years</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Salary not disclosed</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2 months ago</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Freshersworld</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>Web Developer</t>
         </is>

</xml_diff>

<commit_message>
Enhance job listings display by incorporating job descriptions and refining DataFrame formatting for improved clarity and user experience.
</commit_message>
<xml_diff>
--- a/output/jobs.xlsx
+++ b/output/jobs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,36 +484,31 @@
           <t>Job URL</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Searched Job Title</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TECHSHELL SOFTWARE PRIVATE LIMITED</t>
+          <t>Cheerrays Joyful Experiences Private Limited</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TECHSHELL SOFTWARE PRIVATE LIMITED</t>
+          <t>Cheerrays Joyful Experiences Private Limited</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0 Years</t>
+          <t>0 to 0.6 Years</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>240000 - 400000 Yearly</t>
+          <t>10000 - 20000 Monthly</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -528,7 +523,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1 days ago</t>
+          <t>22 days ago</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -539,38 +534,33 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>N/A</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ServiceNow Software Development India Pvt .Ltd</t>
+          <t>TeamLease Services Ltd...</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ServiceNow Software Development India Pvt .Ltd</t>
+          <t>TeamLease Services Ltd...</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3 to 7 Years</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>500000 - 900000 Yearly</t>
+          <t>1000 - 2000 Monthly</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -585,7 +575,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>10 days ago</t>
+          <t>23 hours ago</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -596,38 +586,33 @@
       <c r="J3" t="inlineStr">
         <is>
           <t>N/A</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Accenture Solutions Pvt Ltd</t>
+          <t>Open Text Technologies India Private Limited</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Accenture Solutions Pvt Ltd</t>
+          <t>Open Text Technologies India Private Limited</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4 to 10 Years</t>
+          <t>2 to 4 Years</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>200000 - 700000 Monthly</t>
+          <t>100000 - 170000 Monthly</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -642,7 +627,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>12 days ago</t>
+          <t>3 days ago</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -653,38 +638,33 @@
       <c r="J4" t="inlineStr">
         <is>
           <t>N/A</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>For a Client of TeamLease Digital</t>
+          <t>Biogen Capability Center India Private limited</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>For a Client of TeamLease Digital</t>
+          <t>Biogen Capability Center India Private limited</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2 to 3 Years</t>
+          <t>10 to 15 Years</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>300000 - 600000 Yearly</t>
+          <t>200000 - 400000 Monthly</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -699,7 +679,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>22 days ago</t>
+          <t>3 days ago</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -710,38 +690,33 @@
       <c r="J5" t="inlineStr">
         <is>
           <t>N/A</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Biogen Capability Center India Private limited</t>
+          <t>Smarten Spaces Pte Ltd</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Biogen Capability Center India Private limited</t>
+          <t>Smarten Spaces Pte Ltd</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0 Years</t>
+          <t>6 to 10 Years</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>200000 - 2500000 Monthly</t>
+          <t>200000 - 250000 Monthly</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -756,7 +731,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>3 months ago</t>
+          <t>8 days ago</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -767,23 +742,18 @@
       <c r="J6" t="inlineStr">
         <is>
           <t>N/A</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>NITI TECHNOLOGIES INDIA SOFTWARE</t>
+          <t>Accenture Solutions Pvt Ltd</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>NITI TECHNOLOGIES INDIA SOFTWARE</t>
+          <t>Accenture Solutions Pvt Ltd</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -793,12 +763,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0 Years</t>
+          <t>4 to 10 Years</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>18500 - 85200 Monthly</t>
+          <t>200000 - 700000 Monthly</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -813,7 +783,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>1 days ago</t>
+          <t>12 days ago</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -824,38 +794,33 @@
       <c r="J7" t="inlineStr">
         <is>
           <t>N/A</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ray Business Technologies Pvt Ltd</t>
+          <t>For a Client of TeamLease Digital</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ray Business Technologies Pvt Ltd</t>
+          <t>For a Client of TeamLease Digital</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0 to 0.6 Years</t>
+          <t>0 to 4 Years</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>15000 - 16000 Monthly</t>
+          <t>1000 - 5000000 Monthly</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -870,7 +835,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2 days ago</t>
+          <t>1 months ago</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -881,23 +846,18 @@
       <c r="J8" t="inlineStr">
         <is>
           <t>N/A</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mphasis</t>
+          <t>NITI TECHNOLOGIES INDIA SOFTWARE</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mphasis</t>
+          <t>NITI TECHNOLOGIES INDIA SOFTWARE</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -907,12 +867,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3 Years</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>120000 - 140000 Monthly</t>
+          <t>18500 - 85200 Monthly</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -927,7 +887,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>6 days ago</t>
+          <t>1 days ago</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -938,23 +898,18 @@
       <c r="J9" t="inlineStr">
         <is>
           <t>N/A</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Innasoft Techonologies</t>
+          <t>Mphasis</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Innasoft Techonologies</t>
+          <t>Mphasis</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -964,12 +919,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2 to 2.5 Years</t>
+          <t>3 Years</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>20000 - 50000 Monthly</t>
+          <t>120000 - 140000 Monthly</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -984,7 +939,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1 months ago</t>
+          <t>6 days ago</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -995,38 +950,33 @@
       <c r="J10" t="inlineStr">
         <is>
           <t>N/A</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Digital Jockey</t>
+          <t>Nimblix Technology OPC Pvt LTD</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Digital Jockey</t>
+          <t>Nimblix Technology OPC Pvt LTD</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2 to 3+ Years</t>
+          <t>0 Years</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>15000 - 25000 Monthly</t>
+          <t>25000 - 100000 Monthly</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1041,7 +991,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1 months ago</t>
+          <t>17 days ago</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1052,38 +1002,33 @@
       <c r="J11" t="inlineStr">
         <is>
           <t>N/A</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Apex Web Services</t>
+          <t>EmpowerTec</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Apex Web Services</t>
+          <t>EmpowerTec</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.6 to 1.5 Years</t>
+          <t>0 to 2 Years</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>10000 - 35000 Monthly</t>
+          <t>8000 - 15000 Monthly</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1098,7 +1043,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1 months ago</t>
+          <t>23 days ago</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1109,68 +1054,2294 @@
       <c r="J12" t="inlineStr">
         <is>
           <t>N/A</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>TECHMIYA PROJECTS</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>A Client of Freshersworld</t>
+          <t>TECHMIYA PROJECTS</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
+          <t>0 to 0.6 Years</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>35000 - 40000 Monthly</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>24 days ago</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Right Track Corporate Service</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Right Track Corporate Service</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0.6 to 1 Years</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>30000 - 40000 Monthly</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>1 months ago</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Nimblix Technologies</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Nimblix Technologies</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0 to 3 Years</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>20000 - 40000 Monthly</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>1 months ago</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Freshersworld</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Nimble Solutions Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Nimble Solutions Pvt Ltd</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>0 Years</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Salary not disclosed</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>20000 - 40000 Monthly</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
         <is>
           <t>1 months ago</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>Freshersworld</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Web Developer</t>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>D&amp;A - Consulting</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Ernst &amp; Young</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Competitive stipend</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/d-a-consulting-internship-in-bangalore-at-ernst-young1760617862</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Interim Engineering Intern</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Qualcomm</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Competitive stipend</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/interim-engineering-intern-internship-in-bangalore-at-qualcomm1761507646</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Software Engineering PhD</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Google</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Competitive stipend</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/software-engineering-phd-internship-in-multiple-locations-at-google1760682620</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Silicon Engineering (Hardware) PhD</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Google</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Competitive stipend</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/silicon-engineering-hardware-phd-internship-in-multiple-locations-at-google1760686833</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Network Engineering</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Microsun Infocare Private Limited</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>₹ 11,000 - 17,000 /month</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/network-engineering-internship-in-multiple-locations-at-microsun-infocare-private-limited1764004673</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Mobile App Development</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Uniorbit Technologies Private Limited (Uni Cards)</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>₹ 30,000 - 40,000 /month</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/mobile-app-development-internship-in-bangalore-at-uniorbit-technologies-private-limited-uni-cards1764046445</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Software Development Engineering (Web)</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2xCabs</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>₹ 5,000 - 15,000 /month</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/software-development-engineering-web-internship-in-bangalore-at-2xcabs1763991403</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>iOS App Development</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>NovaFocus Private Limited</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>₹ 18,000 /month</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/ios-app-development-internship-in-bangalore-at-novafocus-private-limited1763974417</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Quality Analyst</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Novora Technology Group</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>₹ 5,000 - 10,000 /month</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/quality-analyst-internship-in-bangalore-at-novora-technology-group1764147572</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Information Security</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Alteryx</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>₹ 85,000 /month</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/information-security-internship-in-bangalore-at-alteryx1764163414</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Web Development</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Rareminds</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>₹ 3,000 - 5,000 /month</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/web-development-internship-in-bangalore-at-rareminds1764081266</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>SaaS Marketing &amp; Sales</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Senso Vision System</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>₹ 5,000 - 10,000 /month</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/saas-marketing-sales-internship-in-bangalore-at-senso-vision-system1763739110</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Software Development Engineering (Web)</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Microsoft</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Competitive stipend</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/software-development-engineering-web-internship-in-bangalore-at-microsoft1762411026</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Full Stack Development</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Wizda Learning Solutions Private Limited</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>₹ 10,000 - 15,000 /month</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-bangalore-at-wizda-learning-solutions-private-limited1764004879</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Full Stack Development</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>HireHunch (HTH Technolabs Private Limited)</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>₹ 13,000 - 15,000 /month</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>1 week ago</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-bangalore-at-hirehunch-hth-technolabs-private-limited1764926324</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Software Developer</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>IBM India Private Limited</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Competitive stipend</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>1 week ago</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/software-developer-internship-in-multiple-locations-at-ibm-india-private-limited1765186692</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Full Stack Development</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Eastencher Software Private Limited</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>₹ 10,000 - 12,000 /month</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>7 days ago</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-bangalore-at-eastencher-software-private-limited1765432965</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Software Development</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>EvenRank</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>₹ 23,000 - 30,000 /month</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>7 days ago</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/software-development-internship-in-bangalore-at-evenrank1765442199</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Full Stack Development</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Chainlink Technology Private Limited</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>₹ 10,000 - 20,000 /month</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>1 week ago</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-bangalore-at-chainlink-technology-private-limited1765178602</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Tech &amp; Marketing Automation</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Chessworld AI</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>₹ 5,000 - 10,000 /month</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/tech-marketing-automation-internship-in-bangalore-at-chessworld-ai1763474356</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Web Development</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Green Lakes</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>₹ 14,000 - 18,000 /month</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2 weeks ago</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/web-development-internship-in-bangalore-at-green-lakes1764594989</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Software Development</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Finplify Technologies Private Limited</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>₹ 5,000 - 12,000 /month</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2 weeks ago</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/software-development-internship-in-bangalore-at-finplify-technologies-private-limited1764860377</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Software Engineering PhD Intern, Summer 2026</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Google</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Competitive stipend</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2 weeks ago</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/software-engineering-phd-intern-summer-2026-internship-in-multiple-locations-at-google1764845633</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Information Technology</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ITGS Infotech Private Limited</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>₹ 10,000 - 20,000 /month</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2 weeks ago</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/part-time-information-technology-internship-in-multiple-locations-at-itgs-infotech-private-limited1764671132</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Information Technology</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Nik Kumari</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>₹ 2,000 - 10,000 /month</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2 weeks ago</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/part-time-information-technology-internship-in-bangalore-at-nik-kumari1764650544</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>WebFlow Developer</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Everything Flow</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>₹ 21,000 /month</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>6 days ago</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/webflow-developer-internship-in-bangalore-at-everything-flow1765535017</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Product Content Writer</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Talview</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>₹ 18,000 - 20,000 /month</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2 weeks ago</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/product-content-writer-internship-in-bangalore-at-talview1764585667</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>iOS App Development</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>TSTEPS PRIVATE LIMITED</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>₹ 30,000 - 40,000 /month</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/ios-app-development-internship-in-multiple-locations-at-tsteps-private-limited1762159806</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Mobile App Development</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Techasoft Private Limited</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>₹ 12,000 - 15,000 /month</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/mobile-app-development-internship-in-multiple-locations-at-techasoft-private-limited1763988484</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Network Engineering</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Wasteland Mineral Private Limited</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>₹ 7,500 - 12,500 /month</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2 weeks ago</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/network-engineering-internship-in-bangalore-at-wasteland-mineral-private-limited1764694092</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Full Stack Development Specific Backend (Laravel)</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>MadeByMaa Food Network Private Limited</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>₹ 5,000 - 8,000 /month</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>1 week ago</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/full-stack-development-specific-backend-laravel-internship-in-bangalore-at-madebymaa-food-network-private-limited1765360904</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Software Testing &amp; Training</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Inland World Logistics Private Limited</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>₹ 20,000 - 25,000 /month</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/software-testing-training-internship-in-bangalore-at-inland-world-logistics-private-limited1764145051</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Photography</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Brandshark</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>₹ 10,000 /month</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2 weeks ago</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/photography-internship-in-bangalore-at-brandshark1764660660</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Graphic Design</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Clippet Technolgies Private Litimed</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>₹ 11,000 - 16,000 /month</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>1 week ago</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/graphic-design-internship-in-bangalore-at-clippet-technolgies-private-litimed1765021806</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Full Stack Development</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Super Health</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>₹ 15,000 /month</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-bangalore-at-super-health1764162499</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Software Development Engineering (Web)</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>PayAssured</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>₹ 5,000 - 10,000 /month</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>3 weeks ago</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/software-development-engineering-web-internship-in-bangalore-at-payassured1763552088</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Backend Development</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Inferigence Quotient Private Limited</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>₹ 20,000 - 30,000 /month</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>1 day ago</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/backend-development-internship-in-bangalore-at-inferigence-quotient-private-limited1765944646</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Cyber Security</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>LI-MAT SOFT SOLUTIONS PRIVATE LIMITED</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>₹ 5,000 - 10,000 /month</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>5 days ago</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/cyber-security-internship-in-bangalore-at-li-mat-soft-solutions-private-limited1765599533</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Presales Engineer</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>LivNSense</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>₹ 10,000 - 15,000 /month</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>7 days ago</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/presales-engineer-internship-in-bangalore-at-livnsense1765443797</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Digital Illustrator</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Dashtoon</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>₹ 10,000 - 15,000 /month</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>6 days ago</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Internshala</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/digital-illustrator-internship-in-bangalore-at-dashtoon1765537999</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor job data extraction and display logic for Freshersworld and Internshala to enhance accuracy, improve error handling, and streamline the presentation of job listings.
</commit_message>
<xml_diff>
--- a/output/jobs.xlsx
+++ b/output/jobs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,27 +488,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cheerrays Joyful Experiences Private Limited</t>
+          <t>D&amp;A - Consulting</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cheerrays Joyful Experiences Private Limited</t>
+          <t>Ernst &amp; Young</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0 to 0.6 Years</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>10000 - 20000 Monthly</t>
+          <t>Competitive stipend</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -523,44 +523,44 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>22 days ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/d-a-consulting-internship-in-bangalore-at-ernst-young1760617862</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TeamLease Services Ltd...</t>
+          <t>Interim Engineering Intern</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TeamLease Services Ltd...</t>
+          <t>Qualcomm</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0 Years</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1000 - 2000 Monthly</t>
+          <t>Competitive stipend</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -575,44 +575,44 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>23 hours ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/interim-engineering-intern-internship-in-bangalore-at-qualcomm1761507646</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Open Text Technologies India Private Limited</t>
+          <t>Software Engineering PhD</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Open Text Technologies India Private Limited</t>
+          <t>Google</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2 to 4 Years</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>100000 - 170000 Monthly</t>
+          <t>Competitive stipend</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -627,44 +627,44 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>3 days ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/software-engineering-phd-internship-in-multiple-locations-at-google1760682620</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Biogen Capability Center India Private limited</t>
+          <t>Silicon Engineering (Hardware) PhD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Biogen Capability Center India Private limited</t>
+          <t>Google</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10 to 15 Years</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>200000 - 400000 Monthly</t>
+          <t>Competitive stipend</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -679,44 +679,44 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>3 days ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/silicon-engineering-hardware-phd-internship-in-multiple-locations-at-google1760686833</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Smarten Spaces Pte Ltd</t>
+          <t>Network Engineering</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Smarten Spaces Pte Ltd</t>
+          <t>Microsun Infocare Private Limited</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>6 to 10 Years</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>200000 - 250000 Monthly</t>
+          <t>₹ 11,000 - 17,000 /month</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -731,44 +731,44 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>8 days ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/network-engineering-internship-in-multiple-locations-at-microsun-infocare-private-limited1764004673</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Accenture Solutions Pvt Ltd</t>
+          <t>Mobile App Development</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Accenture Solutions Pvt Ltd</t>
+          <t>Uniorbit Technologies Private Limited (Uni Cards)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4 to 10 Years</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>200000 - 700000 Monthly</t>
+          <t>₹ 30,000 - 40,000 /month</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -783,44 +783,44 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>12 days ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/mobile-app-development-internship-in-bangalore-at-uniorbit-technologies-private-limited-uni-cards1764046445</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>For a Client of TeamLease Digital</t>
+          <t>Software Development Engineering (Web)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>For a Client of TeamLease Digital</t>
+          <t>2xCabs</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0 to 4 Years</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1000 - 5000000 Monthly</t>
+          <t>₹ 5,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -835,44 +835,44 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>1 months ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/software-development-engineering-web-internship-in-bangalore-at-2xcabs1763991403</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>NITI TECHNOLOGIES INDIA SOFTWARE</t>
+          <t>iOS App Development</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>NITI TECHNOLOGIES INDIA SOFTWARE</t>
+          <t>NovaFocus Private Limited</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0 Years</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>18500 - 85200 Monthly</t>
+          <t>₹ 18,000 /month</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -887,44 +887,44 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>1 days ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/ios-app-development-internship-in-bangalore-at-novafocus-private-limited1763974417</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Mphasis</t>
+          <t>Quality Analyst</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Mphasis</t>
+          <t>Novora Technology Group</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Hyderabad</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3 Years</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>120000 - 140000 Monthly</t>
+          <t>₹ 5,000 - 10,000 /month</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -939,44 +939,44 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>6 days ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/quality-analyst-internship-in-bangalore-at-novora-technology-group1764147572</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Nimblix Technology OPC Pvt LTD</t>
+          <t>Information Security</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Nimblix Technology OPC Pvt LTD</t>
+          <t>Alteryx</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0 Years</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>25000 - 100000 Monthly</t>
+          <t>₹ 85,000 /month</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -991,44 +991,44 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>17 days ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/information-security-internship-in-bangalore-at-alteryx1764163414</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>EmpowerTec</t>
+          <t>Web Development</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>EmpowerTec</t>
+          <t>Rareminds</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0 to 2 Years</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>8000 - 15000 Monthly</t>
+          <t>₹ 3,000 - 5,000 /month</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1043,44 +1043,44 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>23 days ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/web-development-internship-in-bangalore-at-rareminds1764081266</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>TECHMIYA PROJECTS</t>
+          <t>SaaS Marketing &amp; Sales</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TECHMIYA PROJECTS</t>
+          <t>Senso Vision System</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0 to 0.6 Years</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>35000 - 40000 Monthly</t>
+          <t>₹ 5,000 - 10,000 /month</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1095,44 +1095,44 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>24 days ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/saas-marketing-sales-internship-in-bangalore-at-senso-vision-system1763739110</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Right Track Corporate Service</t>
+          <t>Software Development Engineering (Web)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Right Track Corporate Service</t>
+          <t>Microsoft</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.6 to 1 Years</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>30000 - 40000 Monthly</t>
+          <t>Competitive stipend</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1147,44 +1147,44 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1 months ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/software-development-engineering-web-internship-in-bangalore-at-microsoft1762411026</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Nimblix Technologies</t>
+          <t>Full Stack Development</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Nimblix Technologies</t>
+          <t>Wizda Learning Solutions Private Limited</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0 to 3 Years</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>20000 - 40000 Monthly</t>
+          <t>₹ 10,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1199,44 +1199,44 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1 months ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-bangalore-at-wizda-learning-solutions-private-limited1764004879</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Nimble Solutions Pvt Ltd</t>
+          <t>Full Stack Development</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Nimble Solutions Pvt Ltd</t>
+          <t>HireHunch (HTH Technolabs Private Limited)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0 Years</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>20000 - 40000 Monthly</t>
+          <t>₹ 13,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1251,39 +1251,39 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1 months ago</t>
+          <t>1 week ago</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Freshersworld</t>
+          <t>Internshala</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-bangalore-at-hirehunch-hth-technolabs-private-limited1764926324</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>D&amp;A - Consulting</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ernst &amp; Young</t>
+          <t>IBM India Private Limited</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>1 week ago</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1313,34 +1313,34 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/d-a-consulting-internship-in-bangalore-at-ernst-young1760617862</t>
+          <t>https://internshala.com/internship/detail/software-developer-internship-in-multiple-locations-at-ibm-india-private-limited1765186692</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Interim Engineering Intern</t>
+          <t>Full Stack Development</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Qualcomm</t>
+          <t>Eastencher Software Private Limited</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Competitive stipend</t>
+          <t>₹ 10,000 - 12,000 /month</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1355,7 +1355,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>7 days ago</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1365,34 +1365,34 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/interim-engineering-intern-internship-in-bangalore-at-qualcomm1761507646</t>
+          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-bangalore-at-eastencher-software-private-limited1765432965</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Software Engineering PhD</t>
+          <t>Software Development</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Google</t>
+          <t>EvenRank</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Competitive stipend</t>
+          <t>₹ 23,000 - 30,000 /month</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1407,7 +1407,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>7 days ago</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1417,34 +1417,34 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/software-engineering-phd-internship-in-multiple-locations-at-google1760682620</t>
+          <t>https://internshala.com/internship/detail/software-development-internship-in-bangalore-at-evenrank1765442199</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Silicon Engineering (Hardware) PhD</t>
+          <t>Full Stack Development</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Google</t>
+          <t>Chainlink Technology Private Limited</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Competitive stipend</t>
+          <t>₹ 10,000 - 20,000 /month</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1459,7 +1459,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>1 week ago</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1469,34 +1469,34 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/silicon-engineering-hardware-phd-internship-in-multiple-locations-at-google1760686833</t>
+          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-bangalore-at-chainlink-technology-private-limited1765178602</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Network Engineering</t>
+          <t>Tech &amp; Marketing Automation</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Microsun Infocare Private Limited</t>
+          <t>Chessworld AI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>₹ 11,000 - 17,000 /month</t>
+          <t>₹ 5,000 - 10,000 /month</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1521,34 +1521,34 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/network-engineering-internship-in-multiple-locations-at-microsun-infocare-private-limited1764004673</t>
+          <t>https://internshala.com/internship/detail/tech-marketing-automation-internship-in-bangalore-at-chessworld-ai1763474356</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Mobile App Development</t>
+          <t>Web Development</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Uniorbit Technologies Private Limited (Uni Cards)</t>
+          <t>Green Lakes</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>₹ 30,000 - 40,000 /month</t>
+          <t>₹ 14,000 - 18,000 /month</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1563,7 +1563,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1573,34 +1573,34 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/mobile-app-development-internship-in-bangalore-at-uniorbit-technologies-private-limited-uni-cards1764046445</t>
+          <t>https://internshala.com/internship/detail/web-development-internship-in-bangalore-at-green-lakes1764594989</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Software Development Engineering (Web)</t>
+          <t>Software Development</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2xCabs</t>
+          <t>Finplify Technologies Private Limited</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 15,000 /month</t>
+          <t>₹ 5,000 - 12,000 /month</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1615,7 +1615,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1625,34 +1625,34 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/software-development-engineering-web-internship-in-bangalore-at-2xcabs1763991403</t>
+          <t>https://internshala.com/internship/detail/software-development-internship-in-bangalore-at-finplify-technologies-private-limited1764860377</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>iOS App Development</t>
+          <t>Software Engineering PhD Intern, Summer 2026</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>NovaFocus Private Limited</t>
+          <t>Google</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>₹ 18,000 /month</t>
+          <t>Competitive stipend</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1667,7 +1667,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1677,34 +1677,34 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/ios-app-development-internship-in-bangalore-at-novafocus-private-limited1763974417</t>
+          <t>https://internshala.com/internship/detail/software-engineering-phd-intern-summer-2026-internship-in-multiple-locations-at-google1764845633</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Quality Analyst</t>
+          <t>Information Technology</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Novora Technology Group</t>
+          <t>ITGS Infotech Private Limited</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 10,000 /month</t>
+          <t>₹ 10,000 - 20,000 /month</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1719,7 +1719,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1729,34 +1729,34 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/quality-analyst-internship-in-bangalore-at-novora-technology-group1764147572</t>
+          <t>https://internshala.com/internship/detail/part-time-information-technology-internship-in-multiple-locations-at-itgs-infotech-private-limited1764671132</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Information Security</t>
+          <t>Information Technology</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Alteryx</t>
+          <t>Nik Kumari</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>₹ 85,000 /month</t>
+          <t>₹ 2,000 - 10,000 /month</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1771,7 +1771,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1781,34 +1781,34 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/information-security-internship-in-bangalore-at-alteryx1764163414</t>
+          <t>https://internshala.com/internship/detail/part-time-information-technology-internship-in-bangalore-at-nik-kumari1764650544</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Web Development</t>
+          <t>WebFlow Developer</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Rareminds</t>
+          <t>Everything Flow</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>₹ 3,000 - 5,000 /month</t>
+          <t>₹ 21,000 /month</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>6 days ago</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1833,34 +1833,34 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/web-development-internship-in-bangalore-at-rareminds1764081266</t>
+          <t>https://internshala.com/internship/detail/webflow-developer-internship-in-bangalore-at-everything-flow1765535017</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SaaS Marketing &amp; Sales</t>
+          <t>Product Content Writer</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Senso Vision System</t>
+          <t>Talview</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 10,000 /month</t>
+          <t>₹ 18,000 - 20,000 /month</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1875,7 +1875,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -1885,34 +1885,34 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/saas-marketing-sales-internship-in-bangalore-at-senso-vision-system1763739110</t>
+          <t>https://internshala.com/internship/detail/product-content-writer-internship-in-bangalore-at-talview1764585667</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Software Development Engineering (Web)</t>
+          <t>iOS App Development</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Microsoft</t>
+          <t>TSTEPS PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Competitive stipend</t>
+          <t>₹ 30,000 - 40,000 /month</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1937,34 +1937,34 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/software-development-engineering-web-internship-in-bangalore-at-microsoft1762411026</t>
+          <t>https://internshala.com/internship/detail/ios-app-development-internship-in-multiple-locations-at-tsteps-private-limited1762159806</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Full Stack Development</t>
+          <t>Network Engineering</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Wizda Learning Solutions Private Limited</t>
+          <t>Wasteland Mineral Private Limited</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>₹ 10,000 - 15,000 /month</t>
+          <t>₹ 7,500 - 12,500 /month</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -1989,34 +1989,34 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-bangalore-at-wizda-learning-solutions-private-limited1764004879</t>
+          <t>https://internshala.com/internship/detail/network-engineering-internship-in-bangalore-at-wasteland-mineral-private-limited1764694092</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Full Stack Development</t>
+          <t>Full Stack Development Specific Backend (Laravel)</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>HireHunch (HTH Technolabs Private Limited)</t>
+          <t>MadeByMaa Food Network Private Limited</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>₹ 13,000 - 15,000 /month</t>
+          <t>₹ 5,000 - 8,000 /month</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2041,34 +2041,34 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-bangalore-at-hirehunch-hth-technolabs-private-limited1764926324</t>
+          <t>https://internshala.com/internship/detail/full-stack-development-specific-backend-laravel-internship-in-bangalore-at-madebymaa-food-network-private-limited1765360904</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Software Developer</t>
+          <t>Software Testing &amp; Training</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>IBM India Private Limited</t>
+          <t>Inland World Logistics Private Limited</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Competitive stipend</t>
+          <t>₹ 20,000 - 25,000 /month</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1 week ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2093,34 +2093,34 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/software-developer-internship-in-multiple-locations-at-ibm-india-private-limited1765186692</t>
+          <t>https://internshala.com/internship/detail/software-testing-training-internship-in-bangalore-at-inland-world-logistics-private-limited1764145051</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Full Stack Development</t>
+          <t>Photography</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Eastencher Software Private Limited</t>
+          <t>Brandshark</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>₹ 10,000 - 12,000 /month</t>
+          <t>₹ 10,000 /month</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2135,7 +2135,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>7 days ago</t>
+          <t>2 weeks ago</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2145,34 +2145,34 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-bangalore-at-eastencher-software-private-limited1765432965</t>
+          <t>https://internshala.com/internship/detail/photography-internship-in-bangalore-at-brandshark1764660660</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Software Development</t>
+          <t>Graphic Design</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>EvenRank</t>
+          <t>Clippet Technolgies Private Litimed</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>₹ 23,000 - 30,000 /month</t>
+          <t>₹ 11,000 - 16,000 /month</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2187,7 +2187,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>7 days ago</t>
+          <t>1 week ago</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2197,34 +2197,34 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/software-development-internship-in-bangalore-at-evenrank1765442199</t>
+          <t>https://internshala.com/internship/detail/graphic-design-internship-in-bangalore-at-clippet-technolgies-private-litimed1765021806</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Full Stack Development</t>
+          <t>Software Development Engineering (Web)</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Chainlink Technology Private Limited</t>
+          <t>PayAssured</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>₹ 10,000 - 20,000 /month</t>
+          <t>₹ 5,000 - 10,000 /month</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2239,7 +2239,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>1 week ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2249,34 +2249,34 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-bangalore-at-chainlink-technology-private-limited1765178602</t>
+          <t>https://internshala.com/internship/detail/software-development-engineering-web-internship-in-bangalore-at-payassured1763552088</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Tech &amp; Marketing Automation</t>
+          <t>Backend Development</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Chessworld AI</t>
+          <t>Inferigence Quotient Private Limited</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 10,000 /month</t>
+          <t>₹ 20,000 - 30,000 /month</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>3 weeks ago</t>
+          <t>1 day ago</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2301,34 +2301,34 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/tech-marketing-automation-internship-in-bangalore-at-chessworld-ai1763474356</t>
+          <t>https://internshala.com/internship/detail/backend-development-internship-in-bangalore-at-inferigence-quotient-private-limited1765944646</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Web Development</t>
+          <t>Cyber Security</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Green Lakes</t>
+          <t>LI-MAT SOFT SOLUTIONS PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>₹ 14,000 - 18,000 /month</t>
+          <t>₹ 5,000 - 10,000 /month</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2343,7 +2343,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2 weeks ago</t>
+          <t>5 days ago</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2353,34 +2353,34 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/web-development-internship-in-bangalore-at-green-lakes1764594989</t>
+          <t>https://internshala.com/internship/detail/cyber-security-internship-in-bangalore-at-li-mat-soft-solutions-private-limited1765599533</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Software Development</t>
+          <t>Presales Engineer</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Finplify Technologies Private Limited</t>
+          <t>LivNSense</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 12,000 /month</t>
+          <t>₹ 10,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2395,7 +2395,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2 weeks ago</t>
+          <t>7 days ago</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2405,34 +2405,34 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/software-development-internship-in-bangalore-at-finplify-technologies-private-limited1764860377</t>
+          <t>https://internshala.com/internship/detail/presales-engineer-internship-in-bangalore-at-livnsense1765443797</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Software Engineering PhD Intern, Summer 2026</t>
+          <t>Digital Illustrator</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Google</t>
+          <t>Dashtoon</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Competitive stipend</t>
+          <t>₹ 10,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2 weeks ago</t>
+          <t>6 days ago</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2457,34 +2457,34 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/software-engineering-phd-intern-summer-2026-internship-in-multiple-locations-at-google1764845633</t>
+          <t>https://internshala.com/internship/detail/digital-illustrator-internship-in-bangalore-at-dashtoon1765537999</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Information Technology</t>
+          <t>Manual Testing</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ITGS Infotech Private Limited</t>
+          <t>TSTEPS PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>₹ 10,000 - 20,000 /month</t>
+          <t>₹ 30,000 - 40,000 /month</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2499,7 +2499,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2 weeks ago</t>
+          <t>3 weeks ago</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2509,34 +2509,34 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/part-time-information-technology-internship-in-multiple-locations-at-itgs-infotech-private-limited1764671132</t>
+          <t>https://internshala.com/internship/detail/manual-testing-internship-in-multiple-locations-at-tsteps-private-limited1762157179</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Information Technology</t>
+          <t>Java Development</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Nik Kumari</t>
+          <t>Pivotrics Technologies LLP</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Banglore</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Fresher</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>₹ 2,000 - 10,000 /month</t>
+          <t>₹ 20,000 - 30,000 /month</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2561,787 +2561,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/part-time-information-technology-internship-in-bangalore-at-nik-kumari1764650544</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>WebFlow Developer</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Everything Flow</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Fresher</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>₹ 21,000 /month</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>6 days ago</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/webflow-developer-internship-in-bangalore-at-everything-flow1765535017</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Product Content Writer</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Talview</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Fresher</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>₹ 18,000 - 20,000 /month</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>2 weeks ago</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/product-content-writer-internship-in-bangalore-at-talview1764585667</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>iOS App Development</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>TSTEPS PRIVATE LIMITED</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Fresher</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>₹ 30,000 - 40,000 /month</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>3 weeks ago</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/ios-app-development-internship-in-multiple-locations-at-tsteps-private-limited1762159806</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>Mobile App Development</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Techasoft Private Limited</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Fresher</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>₹ 12,000 - 15,000 /month</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>3 weeks ago</t>
-        </is>
-      </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/mobile-app-development-internship-in-multiple-locations-at-techasoft-private-limited1763988484</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Network Engineering</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Wasteland Mineral Private Limited</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Fresher</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>₹ 7,500 - 12,500 /month</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>2 weeks ago</t>
-        </is>
-      </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/network-engineering-internship-in-bangalore-at-wasteland-mineral-private-limited1764694092</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>Full Stack Development Specific Backend (Laravel)</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>MadeByMaa Food Network Private Limited</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Fresher</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>₹ 5,000 - 8,000 /month</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>1 week ago</t>
-        </is>
-      </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/full-stack-development-specific-backend-laravel-internship-in-bangalore-at-madebymaa-food-network-private-limited1765360904</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>Software Testing &amp; Training</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Inland World Logistics Private Limited</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Fresher</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>₹ 20,000 - 25,000 /month</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>3 weeks ago</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/software-testing-training-internship-in-bangalore-at-inland-world-logistics-private-limited1764145051</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>Photography</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Brandshark</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Fresher</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>₹ 10,000 /month</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>2 weeks ago</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/photography-internship-in-bangalore-at-brandshark1764660660</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>Graphic Design</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Clippet Technolgies Private Litimed</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Fresher</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>₹ 11,000 - 16,000 /month</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>1 week ago</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/graphic-design-internship-in-bangalore-at-clippet-technolgies-private-litimed1765021806</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>Full Stack Development</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Super Health</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Fresher</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>₹ 15,000 /month</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>3 weeks ago</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/full-stack-development-internship-in-bangalore-at-super-health1764162499</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Software Development Engineering (Web)</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>PayAssured</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Fresher</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>₹ 5,000 - 10,000 /month</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>3 weeks ago</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/software-development-engineering-web-internship-in-bangalore-at-payassured1763552088</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>Backend Development</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Inferigence Quotient Private Limited</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Fresher</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>₹ 20,000 - 30,000 /month</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>1 day ago</t>
-        </is>
-      </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/backend-development-internship-in-bangalore-at-inferigence-quotient-private-limited1765944646</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>Cyber Security</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>LI-MAT SOFT SOLUTIONS PRIVATE LIMITED</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Fresher</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>₹ 5,000 - 10,000 /month</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>5 days ago</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/cyber-security-internship-in-bangalore-at-li-mat-soft-solutions-private-limited1765599533</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Presales Engineer</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>LivNSense</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>Fresher</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>₹ 10,000 - 15,000 /month</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>7 days ago</t>
-        </is>
-      </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/presales-engineer-internship-in-bangalore-at-livnsense1765443797</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>Digital Illustrator</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Dashtoon</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Fresher</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>₹ 10,000 - 15,000 /month</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>6 days ago</t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>Internshala</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>https://internshala.com/internship/detail/digital-illustrator-internship-in-bangalore-at-dashtoon1765537999</t>
+          <t>https://internshala.com/internship/detail/java-development-internship-in-bangalore-at-pivotrics-technologies-llp1764666209</t>
         </is>
       </c>
     </row>

</xml_diff>